<commit_message>
edit seeder and add mediaDescriptors seeder
</commit_message>
<xml_diff>
--- a/applications/FS.Abp.Demo/aspnet-core/src/FS.Abp.Demo.Domain.Shared/Files/Menus.xlsx
+++ b/applications/FS.Abp.Demo/aspnet-core/src/FS.Abp.Demo.Domain.Shared/Files/Menus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\FS.Works0831\projects\FS.Abp\applications\FS.Abp.Demo\aspnet-core\src\FS.Abp.Demo.Domain.Shared\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CBABD8A-5FBA-4082-AB39-58CF74258F5D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D19F7CAC-654A-42FF-8C62-BF02CF46DA56}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="90">
   <si>
     <t>申辦服務</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -247,10 +247,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>ContentTypeDisplayName</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Value</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -285,9 +281,6 @@
     <t>教授</t>
   </si>
   <si>
-    <t>系主任</t>
-  </si>
-  <si>
     <t>中山大學材料科學博士</t>
   </si>
   <si>
@@ -304,10 +297,6 @@
     <t>hlhuang8423@gmail.com</t>
   </si>
   <si>
-    <t>Index</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>洪篤傑</t>
   </si>
   <si>
@@ -325,6 +314,42 @@
   </si>
   <si>
     <t>副教授</t>
+  </si>
+  <si>
+    <t>Name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sequence</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>照片</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>經歷</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>教授科目</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>研究室</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>榮譽</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>教授、系主任</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>連絡電話</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1197,17 +1222,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CABCAAE-7468-4D61-8CAC-6B1F09BEC032}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.5703125" customWidth="1"/>
     <col min="2" max="2" width="27.5703125" customWidth="1"/>
-    <col min="3" max="3" width="26" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="28.140625" customWidth="1"/>
+    <col min="6" max="6" width="19.7109375" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1218,13 +1246,13 @@
         <v>57</v>
       </c>
       <c r="C1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1" t="s">
         <v>61</v>
       </c>
-      <c r="D1" t="s">
-        <v>77</v>
-      </c>
       <c r="E1" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1235,13 +1263,10 @@
         <v>59</v>
       </c>
       <c r="C2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2" t="s">
-        <v>69</v>
+        <v>83</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1252,13 +1277,13 @@
         <v>59</v>
       </c>
       <c r="C3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3" t="s">
-        <v>70</v>
+        <v>62</v>
+      </c>
+      <c r="D3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1269,13 +1294,13 @@
         <v>59</v>
       </c>
       <c r="C4" t="s">
-        <v>64</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4" t="s">
-        <v>71</v>
+        <v>63</v>
+      </c>
+      <c r="D4" t="s">
+        <v>88</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1286,13 +1311,13 @@
         <v>59</v>
       </c>
       <c r="C5" t="s">
-        <v>65</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5" t="s">
-        <v>72</v>
+        <v>64</v>
+      </c>
+      <c r="D5" t="s">
+        <v>70</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1303,13 +1328,10 @@
         <v>59</v>
       </c>
       <c r="C6" t="s">
-        <v>66</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6" t="s">
-        <v>73</v>
+        <v>84</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1320,13 +1342,10 @@
         <v>59</v>
       </c>
       <c r="C7" t="s">
-        <v>67</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7" t="s">
-        <v>75</v>
+        <v>85</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1337,13 +1356,10 @@
         <v>59</v>
       </c>
       <c r="C8" t="s">
-        <v>68</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8" t="s">
-        <v>76</v>
+        <v>86</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1354,13 +1370,13 @@
         <v>59</v>
       </c>
       <c r="C9" t="s">
-        <v>63</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9" t="s">
-        <v>78</v>
+        <v>65</v>
+      </c>
+      <c r="D9" t="s">
+        <v>71</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1371,13 +1387,13 @@
         <v>59</v>
       </c>
       <c r="C10" t="s">
-        <v>64</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10" t="s">
-        <v>70</v>
+        <v>66</v>
+      </c>
+      <c r="D10" t="s">
+        <v>73</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1388,13 +1404,13 @@
         <v>59</v>
       </c>
       <c r="C11" t="s">
-        <v>65</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11" t="s">
-        <v>79</v>
+        <v>67</v>
+      </c>
+      <c r="D11" t="s">
+        <v>74</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1405,13 +1421,10 @@
         <v>59</v>
       </c>
       <c r="C12" t="s">
-        <v>66</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12" t="s">
-        <v>80</v>
+        <v>87</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1422,13 +1435,10 @@
         <v>59</v>
       </c>
       <c r="C13" t="s">
-        <v>67</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13" t="s">
-        <v>74</v>
+        <v>83</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1439,13 +1449,13 @@
         <v>59</v>
       </c>
       <c r="C14" t="s">
-        <v>68</v>
-      </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="E14" t="s">
-        <v>81</v>
+        <v>62</v>
+      </c>
+      <c r="D14" t="s">
+        <v>75</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -1453,13 +1463,16 @@
         <v>37</v>
       </c>
       <c r="B15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C15" t="s">
         <v>63</v>
       </c>
-      <c r="E15" t="s">
-        <v>82</v>
+      <c r="D15" t="s">
+        <v>69</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -1467,13 +1480,16 @@
         <v>37</v>
       </c>
       <c r="B16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C16" t="s">
         <v>64</v>
       </c>
-      <c r="E16" t="s">
-        <v>83</v>
+      <c r="D16" t="s">
+        <v>76</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1481,13 +1497,185 @@
         <v>37</v>
       </c>
       <c r="B17" t="s">
+        <v>59</v>
+      </c>
+      <c r="C17" t="s">
+        <v>84</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" t="s">
+        <v>59</v>
+      </c>
+      <c r="C18" t="s">
+        <v>85</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" t="s">
+        <v>59</v>
+      </c>
+      <c r="C19" t="s">
+        <v>86</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" t="s">
+        <v>59</v>
+      </c>
+      <c r="C20" t="s">
+        <v>65</v>
+      </c>
+      <c r="D20" t="s">
+        <v>77</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21" t="s">
+        <v>59</v>
+      </c>
+      <c r="C21" t="s">
+        <v>66</v>
+      </c>
+      <c r="D21" t="s">
+        <v>72</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" t="s">
+        <v>59</v>
+      </c>
+      <c r="C22" t="s">
+        <v>67</v>
+      </c>
+      <c r="D22" t="s">
+        <v>78</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>37</v>
+      </c>
+      <c r="B23" t="s">
+        <v>59</v>
+      </c>
+      <c r="C23" t="s">
+        <v>87</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" t="s">
         <v>60</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C24" t="s">
+        <v>83</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>37</v>
+      </c>
+      <c r="B25" t="s">
+        <v>60</v>
+      </c>
+      <c r="C25" t="s">
+        <v>63</v>
+      </c>
+      <c r="D25" t="s">
+        <v>80</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>37</v>
+      </c>
+      <c r="B26" t="s">
+        <v>60</v>
+      </c>
+      <c r="C26" t="s">
+        <v>62</v>
+      </c>
+      <c r="D26" t="s">
+        <v>79</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>37</v>
+      </c>
+      <c r="B27" t="s">
+        <v>60</v>
+      </c>
+      <c r="C27" t="s">
+        <v>89</v>
+      </c>
+      <c r="D27" t="s">
+        <v>72</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>37</v>
+      </c>
+      <c r="B28" t="s">
+        <v>60</v>
+      </c>
+      <c r="C28" t="s">
         <v>67</v>
       </c>
-      <c r="E17" t="s">
-        <v>74</v>
+      <c r="E28">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>